<commit_message>
fim results - initial
</commit_message>
<xml_diff>
--- a/shiny/cache/forecast.xlsx
+++ b/shiny/cache/forecast.xlsx
@@ -20,9 +20,6 @@
     <t xml:space="preserve">variable</t>
   </si>
   <si>
-    <t xml:space="preserve">2024 Q3</t>
-  </si>
-  <si>
     <t xml:space="preserve">2024 Q4</t>
   </si>
   <si>
@@ -45,6 +42,9 @@
   </si>
   <si>
     <t xml:space="preserve">2026 Q3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2026 Q4</t>
   </si>
   <si>
     <t xml:space="preserve">Consumption Grants</t>
@@ -557,31 +557,31 @@
         <v>12</v>
       </c>
       <c r="C2" t="n">
-        <v>461.92733</v>
+        <v>463.5413257</v>
       </c>
       <c r="D2" t="n">
-        <v>467.087025883687</v>
+        <v>447.088159569206</v>
       </c>
       <c r="E2" t="n">
-        <v>450.668796978304</v>
+        <v>442.796289684976</v>
       </c>
       <c r="F2" t="n">
-        <v>446.412208570169</v>
+        <v>445.709739995982</v>
       </c>
       <c r="G2" t="n">
-        <v>449.361288</v>
+        <v>444.7661988</v>
       </c>
       <c r="H2" t="n">
-        <v>448.453726991034</v>
+        <v>447.863487871975</v>
       </c>
       <c r="I2" t="n">
-        <v>451.587350777436</v>
+        <v>448.188295792375</v>
       </c>
       <c r="J2" t="n">
-        <v>451.948851432976</v>
+        <v>452.346923275822</v>
       </c>
       <c r="K2" t="n">
-        <v>456.1445332</v>
+        <v>454.536674</v>
       </c>
     </row>
     <row r="3">
@@ -592,13 +592,13 @@
         <v>14</v>
       </c>
       <c r="C3" t="n">
-        <v>77.681</v>
+        <v>79.275</v>
       </c>
       <c r="D3" t="n">
         <v>79.275</v>
       </c>
       <c r="E3" t="n">
-        <v>79.275</v>
+        <v>75.203</v>
       </c>
       <c r="F3" t="n">
         <v>75.203</v>
@@ -627,31 +627,31 @@
         <v>16</v>
       </c>
       <c r="C4" t="n">
-        <v>1893.4</v>
+        <v>1922</v>
       </c>
       <c r="D4" t="n">
-        <v>1899.39250303085</v>
+        <v>1915.80213881562</v>
       </c>
       <c r="E4" t="n">
-        <v>1905.12639427327</v>
+        <v>1915.49537974805</v>
       </c>
       <c r="F4" t="n">
-        <v>1910.78790980746</v>
+        <v>1921.04530428972</v>
       </c>
       <c r="G4" t="n">
-        <v>1916.32419500381</v>
+        <v>1926.83504223656</v>
       </c>
       <c r="H4" t="n">
-        <v>1922.09970424634</v>
+        <v>1936.90542286818</v>
       </c>
       <c r="I4" t="n">
-        <v>1932.1453361813</v>
+        <v>1947.35251893945</v>
       </c>
       <c r="J4" t="n">
-        <v>1942.56675775017</v>
+        <v>1958.55020912426</v>
       </c>
       <c r="K4" t="n">
-        <v>1953.73692879267</v>
+        <v>1968.55010329008</v>
       </c>
     </row>
     <row r="5">
@@ -662,31 +662,31 @@
         <v>18</v>
       </c>
       <c r="C5" t="n">
-        <v>3141.6</v>
+        <v>3174.7</v>
       </c>
       <c r="D5" t="n">
-        <v>3175.98175838004</v>
+        <v>3204.80183566645</v>
       </c>
       <c r="E5" t="n">
-        <v>3206.09574740905</v>
+        <v>3231.06115711615</v>
       </c>
       <c r="F5" t="n">
-        <v>3232.36567083857</v>
+        <v>3260.58967717546</v>
       </c>
       <c r="G5" t="n">
-        <v>3261.90611278909</v>
+        <v>3291.22060203007</v>
       </c>
       <c r="H5" t="n">
-        <v>3292.54940462156</v>
+        <v>3322.72316165216</v>
       </c>
       <c r="I5" t="n">
-        <v>3324.0646831367</v>
+        <v>3352.0947052084</v>
       </c>
       <c r="J5" t="n">
-        <v>3353.44808520622</v>
+        <v>3382.01967066365</v>
       </c>
       <c r="K5" t="n">
-        <v>3383.38513261417</v>
+        <v>3411.2234432123</v>
       </c>
     </row>
     <row r="6">
@@ -697,31 +697,31 @@
         <v>20</v>
       </c>
       <c r="C6" t="n">
-        <v>90.735</v>
+        <v>93.901</v>
       </c>
       <c r="D6" t="n">
-        <v>97.834</v>
+        <v>93.901</v>
       </c>
       <c r="E6" t="n">
-        <v>97.834</v>
+        <v>85.879</v>
       </c>
       <c r="F6" t="n">
-        <v>89.812</v>
+        <v>85.879</v>
       </c>
       <c r="G6" t="n">
-        <v>89.812</v>
+        <v>90.218</v>
       </c>
       <c r="H6" t="n">
-        <v>94.151</v>
+        <v>88.068</v>
       </c>
       <c r="I6" t="n">
-        <v>92.001</v>
+        <v>88.068</v>
       </c>
       <c r="J6" t="n">
-        <v>92.001</v>
+        <v>88.068</v>
       </c>
       <c r="K6" t="n">
-        <v>92.001</v>
+        <v>88.068</v>
       </c>
     </row>
     <row r="7">
@@ -732,7 +732,7 @@
         <v>22</v>
       </c>
       <c r="C7" t="n">
-        <v>1.365</v>
+        <v>-0.901</v>
       </c>
       <c r="D7" t="n">
         <v>-0.901</v>
@@ -744,10 +744,10 @@
         <v>-0.901</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.901</v>
+        <v>-2.15</v>
       </c>
       <c r="H7" t="n">
-        <v>-2.15</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -767,7 +767,7 @@
         <v>24</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>0.399999999999999</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -837,31 +837,31 @@
         <v>28</v>
       </c>
       <c r="C10" t="n">
-        <v>641.237</v>
+        <v>655.175</v>
       </c>
       <c r="D10" t="n">
-        <v>654.089822291858</v>
+        <v>661.271179816286</v>
       </c>
       <c r="E10" t="n">
-        <v>667.200263905225</v>
+        <v>674.725766162213</v>
       </c>
       <c r="F10" t="n">
-        <v>680.573488508694</v>
+        <v>689.587400692901</v>
       </c>
       <c r="G10" t="n">
-        <v>694.214763270369</v>
+        <v>698.873554348416</v>
       </c>
       <c r="H10" t="n">
-        <v>703.608329262586</v>
+        <v>709.015878706698</v>
       </c>
       <c r="I10" t="n">
-        <v>713.129001572212</v>
+        <v>719.413289541699</v>
       </c>
       <c r="J10" t="n">
-        <v>722.778500101564</v>
+        <v>729.991705539104</v>
       </c>
       <c r="K10" t="n">
-        <v>732.558568025322</v>
+        <v>740.621831915836</v>
       </c>
     </row>
     <row r="11">
@@ -872,31 +872,31 @@
         <v>30</v>
       </c>
       <c r="C11" t="n">
-        <v>932.4</v>
+        <v>957.6</v>
       </c>
       <c r="D11" t="n">
-        <v>951.088833465518</v>
+        <v>967.107196423835</v>
       </c>
       <c r="E11" t="n">
-        <v>970.152262057916</v>
+        <v>986.808063219515</v>
       </c>
       <c r="F11" t="n">
-        <v>989.597794084724</v>
+        <v>1006.91025486723</v>
       </c>
       <c r="G11" t="n">
-        <v>1009.43308834845</v>
+        <v>1021.54071990454</v>
       </c>
       <c r="H11" t="n">
-        <v>1023.09193980453</v>
+        <v>1036.38376645662</v>
       </c>
       <c r="I11" t="n">
-        <v>1036.93561205285</v>
+        <v>1051.44248334533</v>
       </c>
       <c r="J11" t="n">
-        <v>1050.96660594242</v>
+        <v>1066.72000427332</v>
       </c>
       <c r="K11" t="n">
-        <v>1065.18745616178</v>
+        <v>1082.45993400371</v>
       </c>
     </row>
     <row r="12">
@@ -907,31 +907,31 @@
         <v>32</v>
       </c>
       <c r="C12" t="n">
-        <v>1090.2</v>
+        <v>1118.5</v>
       </c>
       <c r="D12" t="n">
-        <v>1116.08378227538</v>
+        <v>1148.744184989</v>
       </c>
       <c r="E12" t="n">
-        <v>1130.29719654266</v>
+        <v>1163.37353203953</v>
       </c>
       <c r="F12" t="n">
-        <v>1144.69161975241</v>
+        <v>1178.18918496906</v>
       </c>
       <c r="G12" t="n">
-        <v>1159.26935706766</v>
+        <v>1195.82078219596</v>
       </c>
       <c r="H12" t="n">
-        <v>1176.61781913306</v>
+        <v>1213.71623621661</v>
       </c>
       <c r="I12" t="n">
-        <v>1194.22590087546</v>
+        <v>1231.87949564704</v>
       </c>
       <c r="J12" t="n">
-        <v>1212.09748750246</v>
+        <v>1250.31456819432</v>
       </c>
       <c r="K12" t="n">
-        <v>1230.23652236378</v>
+        <v>1269.18692299933</v>
       </c>
     </row>
     <row r="13">
@@ -1012,7 +1012,7 @@
         <v>38</v>
       </c>
       <c r="C15" t="n">
-        <v>4.222</v>
+        <v>2.372</v>
       </c>
       <c r="D15" t="n">
         <v>2.372</v>
@@ -1024,10 +1024,10 @@
         <v>2.372</v>
       </c>
       <c r="G15" t="n">
-        <v>2.372</v>
+        <v>0.49</v>
       </c>
       <c r="H15" t="n">
-        <v>0.49</v>
+        <v>0</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -1047,7 +1047,7 @@
         <v>40</v>
       </c>
       <c r="C16" t="n">
-        <v>1.479</v>
+        <v>1.63</v>
       </c>
       <c r="D16" t="n">
         <v>1.63</v>
@@ -1059,10 +1059,10 @@
         <v>1.63</v>
       </c>
       <c r="G16" t="n">
-        <v>1.63</v>
+        <v>1.671</v>
       </c>
       <c r="H16" t="n">
-        <v>1.671</v>
+        <v>0</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
@@ -1082,31 +1082,31 @@
         <v>42</v>
       </c>
       <c r="C17" t="n">
-        <v>2152.199</v>
+        <v>2171.498</v>
       </c>
       <c r="D17" t="n">
-        <v>2160.427</v>
+        <v>2216.251646875</v>
       </c>
       <c r="E17" t="n">
-        <v>2201.992266473</v>
+        <v>2222.951646875</v>
       </c>
       <c r="F17" t="n">
-        <v>2208.692266473</v>
+        <v>2229.651646875</v>
       </c>
       <c r="G17" t="n">
-        <v>2215.392266473</v>
+        <v>2220.112646875</v>
       </c>
       <c r="H17" t="n">
-        <v>2205.853266473</v>
+        <v>2264.21819616788</v>
       </c>
       <c r="I17" t="n">
-        <v>2249.62423907488</v>
+        <v>2270.19019616788</v>
       </c>
       <c r="J17" t="n">
-        <v>2255.59623907488</v>
+        <v>2277.89019616788</v>
       </c>
       <c r="K17" t="n">
-        <v>2263.29623907488</v>
+        <v>2285.59019616788</v>
       </c>
     </row>
     <row r="18">
@@ -1117,31 +1117,31 @@
         <v>44</v>
       </c>
       <c r="C18" t="n">
-        <v>221.505604545001</v>
+        <v>224.743658420665</v>
       </c>
       <c r="D18" t="n">
-        <v>224.743658420665</v>
+        <v>228.029047409692</v>
       </c>
       <c r="E18" t="n">
-        <v>228.029047409692</v>
+        <v>231.362463474923</v>
       </c>
       <c r="F18" t="n">
-        <v>231.362463474923</v>
+        <v>234.744608694576</v>
       </c>
       <c r="G18" t="n">
-        <v>234.744608694576</v>
+        <v>238.176195410118</v>
       </c>
       <c r="H18" t="n">
-        <v>238.176195410118</v>
+        <v>241.657946376297</v>
       </c>
       <c r="I18" t="n">
-        <v>241.657946376297</v>
+        <v>245.190594913367</v>
       </c>
       <c r="J18" t="n">
-        <v>245.190594913367</v>
+        <v>248.77488506154</v>
       </c>
       <c r="K18" t="n">
-        <v>248.77488506154</v>
+        <v>252.41157173769</v>
       </c>
     </row>
     <row r="19">
@@ -1152,31 +1152,31 @@
         <v>46</v>
       </c>
       <c r="C19" t="n">
-        <v>4465</v>
+        <v>4526.3</v>
       </c>
       <c r="D19" t="n">
-        <v>4506.17006477277</v>
+        <v>4599.01056117126</v>
       </c>
       <c r="E19" t="n">
-        <v>4631.67263502736</v>
+        <v>4622.15249842381</v>
       </c>
       <c r="F19" t="n">
-        <v>4655.04739003882</v>
+        <v>4645.50799100346</v>
       </c>
       <c r="G19" t="n">
-        <v>4678.63509016351</v>
+        <v>4669.0771571723</v>
       </c>
       <c r="H19" t="n">
-        <v>4702.43587688976</v>
+        <v>4788.29147684674</v>
       </c>
       <c r="I19" t="n">
-        <v>4848.93834598928</v>
+        <v>4821.14923693197</v>
       </c>
       <c r="J19" t="n">
-        <v>4882.11625114146</v>
+        <v>4854.37939110322</v>
       </c>
       <c r="K19" t="n">
-        <v>4915.66586744915</v>
+        <v>4887.98436710034</v>
       </c>
     </row>
     <row r="20">
@@ -1187,31 +1187,31 @@
         <v>48</v>
       </c>
       <c r="C20" t="n">
-        <v>2477.5</v>
+        <v>2515.1</v>
       </c>
       <c r="D20" t="n">
-        <v>2498.70051302068</v>
+        <v>2529.55898292532</v>
       </c>
       <c r="E20" t="n">
-        <v>2529.15816810511</v>
+        <v>2561.00840480961</v>
       </c>
       <c r="F20" t="n">
-        <v>2560.6019168812</v>
+        <v>2588.01712691122</v>
       </c>
       <c r="G20" t="n">
-        <v>2587.60624358038</v>
+        <v>2614.62275452149</v>
       </c>
       <c r="H20" t="n">
-        <v>2614.20733389807</v>
+        <v>2639.09180766924</v>
       </c>
       <c r="I20" t="n">
-        <v>2638.67223947288</v>
+        <v>2664.54486008583</v>
       </c>
       <c r="J20" t="n">
-        <v>2664.12111126134</v>
+        <v>2687.78303814039</v>
       </c>
       <c r="K20" t="n">
-        <v>2687.35532427355</v>
+        <v>2712.94914769761</v>
       </c>
     </row>
     <row r="21">
@@ -1222,31 +1222,31 @@
         <v>50</v>
       </c>
       <c r="C21" t="n">
-        <v>493.1</v>
+        <v>509.332755158353</v>
       </c>
       <c r="D21" t="n">
-        <v>509.332755158353</v>
+        <v>526.099889428512</v>
       </c>
       <c r="E21" t="n">
-        <v>526.099889428512</v>
+        <v>543.418994465887</v>
       </c>
       <c r="F21" t="n">
-        <v>543.418994465887</v>
+        <v>561.308241039732</v>
       </c>
       <c r="G21" t="n">
-        <v>561.308241039732</v>
+        <v>557.839987860135</v>
       </c>
       <c r="H21" t="n">
-        <v>557.839987860135</v>
+        <v>554.393164581683</v>
       </c>
       <c r="I21" t="n">
-        <v>554.393164581683</v>
+        <v>550.967638791707</v>
       </c>
       <c r="J21" t="n">
-        <v>550.967638791707</v>
+        <v>547.563278895698</v>
       </c>
       <c r="K21" t="n">
-        <v>547.563278895698</v>
+        <v>544.179954112255</v>
       </c>
     </row>
     <row r="22">
@@ -1257,31 +1257,31 @@
         <v>52</v>
       </c>
       <c r="C22" t="n">
-        <v>162.6</v>
+        <v>163.324749650848</v>
       </c>
       <c r="D22" t="n">
-        <v>166.108108108108</v>
+        <v>163.759599441357</v>
       </c>
       <c r="E22" t="n">
-        <v>166.550368550369</v>
+        <v>163.691956140612</v>
       </c>
       <c r="F22" t="n">
-        <v>166.481572481572</v>
+        <v>163.832074406442</v>
       </c>
       <c r="G22" t="n">
-        <v>166.624078624079</v>
+        <v>163.749936112679</v>
       </c>
       <c r="H22" t="n">
-        <v>166.540540540541</v>
+        <v>163.948034350578</v>
       </c>
       <c r="I22" t="n">
-        <v>166.742014742015</v>
+        <v>164.27175586129</v>
       </c>
       <c r="J22" t="n">
-        <v>167.071253071253</v>
+        <v>164.107479273765</v>
       </c>
       <c r="K22" t="n">
-        <v>166.904176904177</v>
+        <v>164.305577511663</v>
       </c>
     </row>
     <row r="23">
@@ -1292,19 +1292,19 @@
         <v>54</v>
       </c>
       <c r="C23" t="n">
-        <v>2.626465</v>
+        <v>2.649835</v>
       </c>
       <c r="D23" t="n">
-        <v>2.649835</v>
+        <v>2.645442</v>
       </c>
       <c r="E23" t="n">
-        <v>2.645442</v>
+        <v>2.6696</v>
       </c>
       <c r="F23" t="n">
-        <v>2.6696</v>
+        <v>2.693006</v>
       </c>
       <c r="G23" t="n">
-        <v>2.693006</v>
+        <v>2.71754</v>
       </c>
       <c r="H23" t="n">
         <v>2.71754</v>
@@ -1313,7 +1313,7 @@
         <v>2.71754</v>
       </c>
       <c r="J23" t="n">
-        <v>2.71754</v>
+        <v>0</v>
       </c>
       <c r="K23" t="n">
         <v>0</v>
@@ -1327,31 +1327,31 @@
         <v>56</v>
       </c>
       <c r="C24" t="n">
-        <v>79.6290028317487</v>
+        <v>71.1791672183253</v>
       </c>
       <c r="D24" t="n">
-        <v>71.1791672183253</v>
+        <v>73.9806362924226</v>
       </c>
       <c r="E24" t="n">
-        <v>73.9806362924226</v>
+        <v>88.3944428040623</v>
       </c>
       <c r="F24" t="n">
-        <v>88.3944428040623</v>
+        <v>103.083510693309</v>
       </c>
       <c r="G24" t="n">
-        <v>103.083510693309</v>
+        <v>109.658761987664</v>
       </c>
       <c r="H24" t="n">
-        <v>109.658761987664</v>
+        <v>134.709036355557</v>
       </c>
       <c r="I24" t="n">
-        <v>134.709036355557</v>
+        <v>155.206844624839</v>
       </c>
       <c r="J24" t="n">
-        <v>155.206844624839</v>
+        <v>162.820344255939</v>
       </c>
       <c r="K24" t="n">
-        <v>162.820344255939</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>